<commit_message>
lots of transition data that may need filtering
</commit_message>
<xml_diff>
--- a/03_Water_Quality/0301_EMC_values_from_literature_and_database.xlsx
+++ b/03_Water_Quality/0301_EMC_values_from_literature_and_database.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://niva365-my.sharepoint.com/personal/astha_bista_niva_no/Documents/Documents/GitHub/SWMM_MOO/03_Water_Quality/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="8_{859A4391-BE37-45F3-901A-97701437B5CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1F09377E-70F7-4663-9DE5-483260546F9A}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="8_{859A4391-BE37-45F3-901A-97701437B5CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{93588DC6-CEDE-4E42-8623-A2F5ECD038E6}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{83A3BA3F-9A17-4080-9E89-85881927B0C9}"/>
+    <workbookView xWindow="10260" yWindow="2055" windowWidth="17280" windowHeight="9105" xr2:uid="{83A3BA3F-9A17-4080-9E89-85881927B0C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Equar" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,6 +42,7 @@
   <authors>
     <author>tc={C009BC56-1CB9-4A7D-B9AB-720A404CD3CC}</author>
     <author>tc={71793F32-28D1-40C1-9958-18A351B39AC4}</author>
+    <author>tc={2312EC27-B161-4D7A-A0AB-B78DCE76BB11}</author>
   </authors>
   <commentList>
     <comment ref="F1" authorId="0" shapeId="0" xr:uid="{C009BC56-1CB9-4A7D-B9AB-720A404CD3CC}">
@@ -59,12 +61,20 @@
     Assumed 0. But maybe find source.</t>
       </text>
     </comment>
+    <comment ref="N4" authorId="2" shapeId="0" xr:uid="{2312EC27-B161-4D7A-A0AB-B78DCE76BB11}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Assumed 0. But maybe find source.</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
   <si>
     <t>BC</t>
   </si>
@@ -112,6 +122,18 @@
   </si>
   <si>
     <t xml:space="preserve">Further details: </t>
+  </si>
+  <si>
+    <t>traditional roof</t>
+  </si>
+  <si>
+    <t>Green roof</t>
+  </si>
+  <si>
+    <t>from StormTac</t>
+  </si>
+  <si>
+    <t>From US BMP database</t>
   </si>
 </sst>
 </file>
@@ -145,7 +167,7 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -156,7 +178,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -179,19 +201,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -540,40 +580,49 @@
   <threadedComment ref="D3" dT="2025-06-16T11:30:28.04" personId="{122255F6-D1A5-49AC-A14D-0497E496A421}" id="{71793F32-28D1-40C1-9958-18A351B39AC4}">
     <text>Assumed 0. But maybe find source.</text>
   </threadedComment>
+  <threadedComment ref="N4" dT="2025-06-16T11:30:28.04" personId="{122255F6-D1A5-49AC-A14D-0497E496A421}" id="{2312EC27-B161-4D7A-A0AB-B78DCE76BB11}">
+    <text>Assumed 0. But maybe find source.</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CAD8BA-D360-41A7-B259-CC0360814070}">
-  <dimension ref="A1:U8"/>
+  <dimension ref="A1:U9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T8" sqref="T8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="20" max="20" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2" t="s">
+      <c r="E1" s="3"/>
+      <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2" t="s">
+      <c r="G1" s="3"/>
+      <c r="H1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="2"/>
+      <c r="I1" s="3"/>
+      <c r="K1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" t="s">
+        <v>19</v>
+      </c>
       <c r="T1" t="s">
         <v>15</v>
       </c>
@@ -581,7 +630,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>4</v>
@@ -607,6 +656,16 @@
       <c r="I2" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="K2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="O2" s="3"/>
       <c r="T2" t="s">
         <v>13</v>
       </c>
@@ -614,176 +673,257 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>46</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>10</v>
       </c>
-      <c r="D3" s="3">
-        <v>0</v>
-      </c>
-      <c r="E3" s="3">
+      <c r="D3" s="2">
+        <v>22</v>
+      </c>
+      <c r="E3" s="2">
+        <v>19</v>
+      </c>
+      <c r="F3" s="2">
+        <v>100</v>
+      </c>
+      <c r="G3" s="2">
+        <v>36</v>
+      </c>
+      <c r="H3" s="2">
+        <v>49</v>
+      </c>
+      <c r="I3" s="2">
+        <v>22</v>
+      </c>
+      <c r="K3" s="5">
+        <v>22</v>
+      </c>
+      <c r="L3" s="5">
+        <v>19</v>
+      </c>
+      <c r="N3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="3">
-        <v>100</v>
-      </c>
-      <c r="G3" s="3">
-        <v>36</v>
-      </c>
-      <c r="H3" s="3">
-        <v>49</v>
-      </c>
-      <c r="I3" s="3">
-        <v>22</v>
+      <c r="O3" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>0.22</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>0.2</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3">
-        <v>0.42</v>
-      </c>
-      <c r="F4" s="3">
+      <c r="D4" s="2">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="E4" s="2">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="F4" s="2">
         <v>0.26</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="2">
         <v>0.13</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="2">
         <v>0.17</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="2">
         <v>0.21</v>
       </c>
+      <c r="K4" s="5">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="L4" s="5">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="N4" s="2">
+        <v>0</v>
+      </c>
+      <c r="O4" s="2">
+        <v>4</v>
+      </c>
     </row>
-    <row r="5" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>1.35</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>0.81499999999999995</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3">
-        <v>1.8660000000000001</v>
-      </c>
-      <c r="F5" s="3">
+      <c r="D5" s="2">
+        <v>1.7</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1.8</v>
+      </c>
+      <c r="F5" s="2">
         <v>2</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="2">
         <v>1.5</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="2">
         <v>1.474</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5" s="2">
         <v>1.27</v>
       </c>
+      <c r="K5" s="5">
+        <v>1.7</v>
+      </c>
+      <c r="L5" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2">
+        <v>0.42</v>
+      </c>
     </row>
-    <row r="6" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>7.11E-3</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3">
-        <v>2.2800000000000001E-2</v>
-      </c>
-      <c r="F6" s="3">
+      <c r="D6" s="2">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1.6E-2</v>
+      </c>
+      <c r="F6" s="2">
         <v>0.03</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="2">
         <v>0.02</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="2">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="2">
         <v>9.9000000000000008E-3</v>
       </c>
+      <c r="K6" s="6">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="L6" s="6">
+        <v>1.6E-2</v>
+      </c>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2">
+        <v>1.8660000000000001</v>
+      </c>
     </row>
-    <row r="7" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>5.8999999999999999E-3</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>1.42E-3</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3">
-        <v>6.7000000000000002E-4</v>
-      </c>
-      <c r="F7" s="3">
+      <c r="D7" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="F7" s="2">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="2">
         <v>6.1999999999999998E-3</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="2">
         <v>0.01</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7" s="2">
         <v>4.4999999999999997E-3</v>
       </c>
+      <c r="K7" s="6">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L7" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2">
+        <v>2.2800000000000001E-2</v>
+      </c>
     </row>
-    <row r="8" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="2">
         <v>6.2399999999999997E-2</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <v>1.35E-2</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3">
+      <c r="D8" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="E8" s="2">
+        <v>2.3E-2</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="G8" s="2">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0.10249999999999999</v>
+      </c>
+      <c r="I8" s="2">
+        <v>3.4299999999999997E-2</v>
+      </c>
+      <c r="K8" s="6">
+        <v>0.08</v>
+      </c>
+      <c r="L8" s="6">
+        <v>2.3E-2</v>
+      </c>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2">
+        <v>6.7000000000000002E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="N9" s="2"/>
+      <c r="O9" s="2">
         <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="F8" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="G8" s="3">
-        <v>5.8999999999999997E-2</v>
-      </c>
-      <c r="H8" s="3">
-        <v>0.10249999999999999</v>
-      </c>
-      <c r="I8" s="3">
-        <v>3.4299999999999997E-2</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="H1:I1"/>
+    <mergeCell ref="N2:O2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -794,11 +934,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B058C721-7DBC-4A14-83EF-801761393982}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K49" sqref="K49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>